<commit_message>
Update Notes for SQL Server
</commit_message>
<xml_diff>
--- a/SQL/SQL Server/where-operators.xlsx
+++ b/SQL/SQL Server/where-operators.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8F1F7B-A771-4B80-A72E-6E1213CC7C33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1D7CEE-5B23-4515-9C02-0BC2331F3A20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>`WHERE col_name BETWEEN val_one AND val_two`</t>
   </si>
   <si>
-    <t>Search for a pattern. % and _ are wildcards. `%` is like `+` In regex(0/1/1+).  `_` is like `.`.</t>
-  </si>
-  <si>
     <t>`WHERE col_name IN (val1, val2, val3)`  returns results where col_name is equal to one of the vals. You can also pass in a `(SELECT statement)` instead of` (val1, val2, val3)`.</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>`WHERE col_name IS NULL`</t>
+  </si>
+  <si>
+    <t>Search for a pattern. % and _ are wildcards. `%` is like `+` In regex(0/1/1+).  `_` is like `.`. Also has `[abc]` and `[^abc]` like regex.</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,10 +531,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -545,51 +545,51 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>